<commit_message>
Updated comments to calculation_for_allocation_of_images.xlsx file
</commit_message>
<xml_diff>
--- a/Calculation_for_Allocation_of_Images.xlsx
+++ b/Calculation_for_Allocation_of_Images.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitHub\Malaria-Detector-CNN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitHub\Malaria-Detector-CNN\Allocation of Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDAB6AC-A87A-4BA8-8140-E36369D332B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BD7FCD-7787-4568-81C1-1AB7765FDF2E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="17690" windowHeight="11020" xr2:uid="{5CF980F8-5083-4923-9DA0-07D7FCE332D6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="17930" windowHeight="11020" xr2:uid="{5CF980F8-5083-4923-9DA0-07D7FCE332D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculations" sheetId="1" r:id="rId1"/>
@@ -30,47 +30,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Test</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>SK</t>
-  </si>
-  <si>
     <t>Train</t>
   </si>
   <si>
     <t>Valid</t>
   </si>
   <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t>Skin Cancer Project</t>
-  </si>
-  <si>
     <t>Malaria Project</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
     <t>Desired %</t>
   </si>
   <si>
-    <t>Total Images</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -78,6 +54,15 @@
   </si>
   <si>
     <t>Actual Allocation</t>
+  </si>
+  <si>
+    <t>Parasitized</t>
+  </si>
+  <si>
+    <t>Uninfected</t>
+  </si>
+  <si>
+    <t>Total Images per Category -&gt;</t>
   </si>
 </sst>
 </file>
@@ -113,9 +98,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,271 +420,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6D3ACB-484C-4498-A6AA-E69954DDF94C}">
-  <dimension ref="B1:N16"/>
+  <dimension ref="B1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.6328125" customWidth="1"/>
+    <col min="3" max="3" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1">
+        <v>13779</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1">
-        <v>13779</v>
-      </c>
-    </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="L2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E3" s="1">
+        <f>D3*E$1</f>
+        <v>2755.8</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2756</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E4" s="1">
+        <f>D4*E$1</f>
+        <v>2755.8</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2756</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="D3">
-        <v>117</v>
-      </c>
-      <c r="J3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" ref="E7:E8" si="0">D7*E$1</f>
+        <v>9645.2999999999993</v>
+      </c>
+      <c r="F7" s="1">
+        <v>9645</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="L3">
-        <v>0.2</v>
-      </c>
-      <c r="M3">
-        <f>L3*M$1</f>
-        <v>2755.8</v>
-      </c>
-      <c r="N3">
-        <v>2756</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>393</v>
-      </c>
-      <c r="K4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4">
-        <v>0.2</v>
-      </c>
-      <c r="M4">
-        <f>L4*M$1</f>
-        <v>2755.8</v>
-      </c>
-      <c r="N4">
-        <v>2756</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="F6">
-        <f>SUM(D3:D5)</f>
-        <v>600</v>
-      </c>
-      <c r="G6" s="1">
-        <f>F6/F$16</f>
-        <v>0.21818181818181817</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>374</v>
-      </c>
-      <c r="J7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L7">
+      <c r="D8" s="2">
         <v>0.7</v>
       </c>
-      <c r="M7">
-        <f t="shared" ref="M7:M8" si="0">L7*M$1</f>
-        <v>9645.2999999999993</v>
-      </c>
-      <c r="N7">
-        <v>9645</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>1372</v>
-      </c>
-      <c r="K8" t="s">
-        <v>10</v>
-      </c>
-      <c r="L8">
-        <v>0.7</v>
-      </c>
-      <c r="M8">
+      <c r="E8" s="1">
         <f t="shared" si="0"/>
         <v>9645.2999999999993</v>
       </c>
-      <c r="N8">
+      <c r="F8" s="1">
         <v>9645</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="F10">
-        <f>SUM(D7:D9)</f>
-        <v>2000</v>
-      </c>
-      <c r="G10" s="1">
-        <f>F10/F$16</f>
-        <v>0.72727272727272729</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>30</v>
-      </c>
-      <c r="J11" t="s">
-        <v>5</v>
-      </c>
-      <c r="K11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" ref="E11:E12" si="1">D11*E$1</f>
+        <v>1377.9</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="L11">
+      <c r="D12" s="2">
         <v>0.1</v>
       </c>
-      <c r="M11">
-        <f t="shared" ref="M11:M12" si="1">L11*M$1</f>
-        <v>1377.9</v>
-      </c>
-      <c r="N11">
-        <v>1378</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="C12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>78</v>
-      </c>
-      <c r="K12" t="s">
-        <v>10</v>
-      </c>
-      <c r="L12">
-        <v>0.1</v>
-      </c>
-      <c r="M12">
+      <c r="E12" s="1">
         <f t="shared" si="1"/>
         <v>1377.9</v>
       </c>
-      <c r="N12">
+      <c r="F12" s="1">
         <v>1378</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="F14">
-        <f>SUM(D11:D13)</f>
-        <v>150</v>
-      </c>
-      <c r="G14" s="1">
-        <f>F14/F$16</f>
-        <v>5.4545454545454543E-2</v>
-      </c>
-      <c r="J14" t="s">
-        <v>13</v>
-      </c>
-      <c r="K14" t="s">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1">
+        <f>E3+E7+E11</f>
+        <v>13778.999999999998</v>
+      </c>
+      <c r="F14" s="1">
+        <f>F3+F7+F11</f>
+        <v>13779</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="M14">
-        <f>M3+M7+M11</f>
+      <c r="E15" s="1">
+        <f>E4+E8+E12</f>
         <v>13778.999999999998</v>
       </c>
-      <c r="N14">
-        <f>N3+N7+N11</f>
+      <c r="F15" s="1">
+        <f>F4+F8+F12</f>
         <v>13779</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="K15" t="s">
-        <v>10</v>
-      </c>
-      <c r="M15">
-        <f>M4+M8+M12</f>
-        <v>13778.999999999998</v>
-      </c>
-      <c r="N15">
-        <f>N4+N8+N12</f>
-        <v>13779</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="E16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16">
-        <f>SUM(F3:F15)</f>
-        <v>2750</v>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="1">
+        <f>SUM(E14:E16)</f>
+        <v>27557.999999999996</v>
+      </c>
+      <c r="F17" s="1">
+        <f>SUM(F14:F16)</f>
+        <v>27558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>